<commit_message>
mx_manip : print fn to be reviewed. To complicated, think about inverting the chars array to simplify it.
</commit_message>
<xml_diff>
--- a/refFiles/mx_manip/posRecovery().xlsx
+++ b/refFiles/mx_manip/posRecovery().xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOUGNON-PEIGNE\Documents\_CodePro\SilProj\dev-ws2812b\00-Archives\Matrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOUGNON-PEIGNE\Documents\_CodePro\SilProj\dev-ws2812b\refFiles\mx_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D034D63-768D-4215-A34F-85F8C2EF3F03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1846406B-8644-4AAE-B384-B3233961FACA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="450" windowWidth="12705" windowHeight="11865" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
   </bookViews>
   <sheets>
     <sheet name="0_360" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>Simple Matrix</t>
   </si>
@@ -122,12 +122,21 @@
   <si>
     <t>((X - 1) * MAX_LINE) + (Y - 1)</t>
   </si>
+  <si>
+    <t>i &lt;- 0 to MAX_LINE</t>
+  </si>
+  <si>
+    <t>j &lt;- 0 to MAX_COL</t>
+  </si>
+  <si>
+    <t>i * MAX_COL + j</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +144,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +189,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5B93D0-ABDB-40CB-8D7C-2E1071F7F2BA}">
-  <dimension ref="A1:AH37"/>
+  <dimension ref="A1:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AP10" sqref="AP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,10 +597,12 @@
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
     <col min="19" max="34" width="5.140625" style="2" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="2"/>
+    <col min="35" max="35" width="5.5703125" style="2" customWidth="1"/>
+    <col min="36" max="39" width="5.140625" style="2" customWidth="1"/>
+    <col min="40" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -564,7 +620,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <f t="shared" ref="B2:O2" si="0">C2+1</f>
         <v>255</v>
@@ -693,8 +749,26 @@
         <f t="shared" ref="AH2:AH16" si="16">Q2+256</f>
         <v>496</v>
       </c>
-    </row>
-    <row r="3" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="11">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="8">
+        <v>7</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <f>B4+1</f>
         <v>224</v>
@@ -823,8 +897,16 @@
         <f t="shared" si="16"/>
         <v>495</v>
       </c>
-    </row>
-    <row r="4" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="8"/>
+      <c r="AP3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f t="shared" ref="B4:O4" si="18">C4+1</f>
         <v>223</v>
@@ -953,8 +1035,14 @@
         <f t="shared" si="16"/>
         <v>464</v>
       </c>
-    </row>
-    <row r="5" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="8"/>
+      <c r="AQ4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <f>B6+1</f>
         <v>192</v>
@@ -1083,8 +1171,11 @@
         <f t="shared" si="16"/>
         <v>463</v>
       </c>
-    </row>
-    <row r="6" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="8"/>
+    </row>
+    <row r="6" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" ref="B6:O6" si="20">C6+1</f>
         <v>191</v>
@@ -1213,8 +1304,13 @@
         <f t="shared" si="16"/>
         <v>432</v>
       </c>
-    </row>
-    <row r="7" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="8"/>
+    </row>
+    <row r="7" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f>B8+1</f>
         <v>160</v>
@@ -1343,8 +1439,13 @@
         <f t="shared" si="16"/>
         <v>431</v>
       </c>
-    </row>
-    <row r="8" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="4"/>
+      <c r="AM7" s="4">
+        <v>23</v>
+      </c>
+      <c r="AN7" s="8"/>
+    </row>
+    <row r="8" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" ref="B8:O8" si="22">C8+1</f>
         <v>159</v>
@@ -1473,8 +1574,21 @@
         <f t="shared" si="16"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="9" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="12">
+        <v>24</v>
+      </c>
+      <c r="AK8" s="7">
+        <v>25</v>
+      </c>
+      <c r="AL8" s="7">
+        <v>26</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>27</v>
+      </c>
+      <c r="AN8" s="8"/>
+    </row>
+    <row r="9" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f>B10+1</f>
         <v>128</v>
@@ -1603,8 +1717,14 @@
         <f t="shared" si="16"/>
         <v>399</v>
       </c>
-    </row>
-    <row r="10" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ9" s="8">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+    </row>
+    <row r="10" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" ref="B10:O10" si="24">C10+1</f>
         <v>127</v>
@@ -1733,8 +1853,23 @@
         <f t="shared" si="16"/>
         <v>368</v>
       </c>
-    </row>
-    <row r="11" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="14">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="14">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN10" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f>B12+1</f>
         <v>96</v>
@@ -1863,8 +1998,13 @@
         <f t="shared" si="16"/>
         <v>367</v>
       </c>
-    </row>
-    <row r="12" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ11" s="10">
+        <v>4</v>
+      </c>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="8"/>
+    </row>
+    <row r="12" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" ref="B12:O12" si="26">C12+1</f>
         <v>95</v>
@@ -1993,8 +2133,13 @@
         <f t="shared" si="16"/>
         <v>336</v>
       </c>
-    </row>
-    <row r="13" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="8"/>
+    </row>
+    <row r="13" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f>B14+1</f>
         <v>64</v>
@@ -2123,8 +2268,11 @@
         <f t="shared" si="16"/>
         <v>335</v>
       </c>
-    </row>
-    <row r="14" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="8"/>
+    </row>
+    <row r="14" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" ref="B14:O16" si="28">C14+1</f>
         <v>63</v>
@@ -2253,8 +2401,11 @@
         <f t="shared" si="16"/>
         <v>304</v>
       </c>
-    </row>
-    <row r="15" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ14" s="4"/>
+      <c r="AM14" s="4"/>
+      <c r="AN14" s="8"/>
+    </row>
+    <row r="15" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f>B16+1</f>
         <v>32</v>
@@ -2383,8 +2534,13 @@
         <f t="shared" si="16"/>
         <v>303</v>
       </c>
-    </row>
-    <row r="16" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ15" s="4"/>
+      <c r="AM15" s="4">
+        <v>23</v>
+      </c>
+      <c r="AN15" s="8"/>
+    </row>
+    <row r="16" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="28"/>
         <v>31</v>
@@ -2513,6 +2669,19 @@
         <f t="shared" si="16"/>
         <v>272</v>
       </c>
+      <c r="AJ16" s="2">
+        <v>24</v>
+      </c>
+      <c r="AK16" s="13">
+        <v>25</v>
+      </c>
+      <c r="AL16" s="13">
+        <v>26</v>
+      </c>
+      <c r="AM16">
+        <v>27</v>
+      </c>
+      <c r="AN16" s="8"/>
     </row>
     <row r="17" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -2775,6 +2944,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="AN2:AN8"/>
+    <mergeCell ref="AJ9:AM9"/>
+    <mergeCell ref="AN10:AN16"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2:Q17">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>$F$24</formula>
@@ -2792,10 +2966,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFE2C2D-56A6-462B-9FCF-1302A82E64E8}">
-  <dimension ref="A1:AH30"/>
+  <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2803,10 +2977,14 @@
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
     <col min="19" max="34" width="5.140625" style="2" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="2"/>
+    <col min="35" max="35" width="5.5703125" style="2" customWidth="1"/>
+    <col min="36" max="39" width="5.140625" style="2" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="2"/>
+    <col min="41" max="41" width="9.140625" style="2" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2824,7 +3002,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <f>C2+1</f>
         <v>240</v>
@@ -2953,8 +3131,23 @@
         <f t="shared" si="8"/>
         <v>271</v>
       </c>
-    </row>
-    <row r="3" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="11">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <f>B2+1</f>
         <v>241</v>
@@ -3083,8 +3276,13 @@
         <f t="shared" si="8"/>
         <v>270</v>
       </c>
-    </row>
-    <row r="4" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="8"/>
+    </row>
+    <row r="4" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f t="shared" ref="B4:B17" si="9">B3+1</f>
         <v>242</v>
@@ -3213,8 +3411,11 @@
         <f t="shared" si="8"/>
         <v>269</v>
       </c>
-    </row>
-    <row r="5" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="8"/>
+    </row>
+    <row r="5" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <f t="shared" si="9"/>
         <v>243</v>
@@ -3343,8 +3544,11 @@
         <f t="shared" si="8"/>
         <v>268</v>
       </c>
-    </row>
-    <row r="6" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="8"/>
+    </row>
+    <row r="6" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" si="9"/>
         <v>244</v>
@@ -3473,8 +3677,13 @@
         <f t="shared" si="8"/>
         <v>267</v>
       </c>
-    </row>
-    <row r="7" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="8"/>
+    </row>
+    <row r="7" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" si="9"/>
         <v>245</v>
@@ -3603,8 +3812,13 @@
         <f t="shared" si="8"/>
         <v>266</v>
       </c>
-    </row>
-    <row r="8" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="4"/>
+      <c r="AM7" s="4">
+        <v>23</v>
+      </c>
+      <c r="AN7" s="8"/>
+    </row>
+    <row r="8" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" si="9"/>
         <v>246</v>
@@ -3733,8 +3947,21 @@
         <f t="shared" si="8"/>
         <v>265</v>
       </c>
-    </row>
-    <row r="9" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="12">
+        <v>24</v>
+      </c>
+      <c r="AK8" s="7">
+        <v>25</v>
+      </c>
+      <c r="AL8" s="7">
+        <v>26</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>27</v>
+      </c>
+      <c r="AN8" s="8"/>
+    </row>
+    <row r="9" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" si="9"/>
         <v>247</v>
@@ -3863,8 +4090,14 @@
         <f t="shared" si="8"/>
         <v>264</v>
       </c>
-    </row>
-    <row r="10" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ9" s="8">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+    </row>
+    <row r="10" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="9"/>
         <v>248</v>
@@ -3994,7 +4227,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="9"/>
         <v>249</v>
@@ -4124,7 +4357,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="9"/>
         <v>250</v>
@@ -4254,7 +4487,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="9"/>
         <v>251</v>
@@ -4384,7 +4617,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" si="9"/>
         <v>252</v>
@@ -4514,7 +4747,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f t="shared" si="9"/>
         <v>253</v>
@@ -4644,7 +4877,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="9"/>
         <v>254</v>
@@ -4994,6 +5227,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AN2:AN8"/>
+    <mergeCell ref="AJ9:AM9"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2:Q17">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$F$24</formula>

</xml_diff>

<commit_message>
mx : Reflexion printing char. added to excel.
</commit_message>
<xml_diff>
--- a/refFiles/mx_manip/posRecovery().xlsx
+++ b/refFiles/mx_manip/posRecovery().xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOUGNON-PEIGNE\Documents\_CodePro\SilProj\dev-ws2812b\refFiles\mx_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1846406B-8644-4AAE-B384-B3233961FACA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA8DCE0-793F-4FE8-A645-2D930A180135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
   </bookViews>
   <sheets>
     <sheet name="0_360" sheetId="1" r:id="rId1"/>
     <sheet name="90_-270" sheetId="5" r:id="rId2"/>
     <sheet name="180_-180" sheetId="6" r:id="rId3"/>
     <sheet name="270_-90" sheetId="7" r:id="rId4"/>
+    <sheet name="Refl._Char" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>Simple Matrix</t>
   </si>
@@ -131,12 +132,27 @@
   <si>
     <t>i * MAX_COL + j</t>
   </si>
+  <si>
+    <t>PRINT_MATRIX</t>
+  </si>
+  <si>
+    <t>Identify char</t>
+  </si>
+  <si>
+    <t>Identify WidthXHeight</t>
+  </si>
+  <si>
+    <t>Filling displayArray</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +163,14 @@
     <font>
       <b/>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -179,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,21 +215,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -218,14 +227,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -243,6 +284,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -588,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5B93D0-ABDB-40CB-8D7C-2E1071F7F2BA}">
   <dimension ref="A1:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP10" sqref="AP10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,19 +820,19 @@
         <f t="shared" ref="AH2:AH16" si="16">Q2+256</f>
         <v>496</v>
       </c>
-      <c r="AJ2" s="6">
+      <c r="AJ2" s="5">
         <v>0</v>
       </c>
-      <c r="AK2" s="11">
+      <c r="AK2" s="6">
         <v>1</v>
       </c>
-      <c r="AL2" s="11">
+      <c r="AL2" s="6">
         <v>2</v>
       </c>
-      <c r="AM2" s="5">
+      <c r="AM2" s="12">
         <v>3</v>
       </c>
-      <c r="AN2" s="8">
+      <c r="AN2" s="9">
         <v>7</v>
       </c>
       <c r="AO2" t="s">
@@ -897,11 +968,13 @@
         <f t="shared" si="16"/>
         <v>495</v>
       </c>
-      <c r="AJ3" s="10">
+      <c r="AJ3" s="5">
         <v>4</v>
       </c>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
       <c r="AM3" s="4"/>
-      <c r="AN3" s="8"/>
+      <c r="AN3" s="9"/>
       <c r="AP3" t="s">
         <v>29</v>
       </c>
@@ -1036,8 +1109,10 @@
         <v>464</v>
       </c>
       <c r="AJ4" s="4"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
       <c r="AM4" s="4"/>
-      <c r="AN4" s="8"/>
+      <c r="AN4" s="9"/>
       <c r="AQ4" t="s">
         <v>30</v>
       </c>
@@ -1172,8 +1247,10 @@
         <v>463</v>
       </c>
       <c r="AJ5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="8"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="9"/>
     </row>
     <row r="6" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -1305,10 +1382,10 @@
         <v>432</v>
       </c>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="8"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="9"/>
     </row>
     <row r="7" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -1440,10 +1517,12 @@
         <v>431</v>
       </c>
       <c r="AJ7" s="4"/>
-      <c r="AM7" s="4">
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13">
         <v>23</v>
       </c>
-      <c r="AN7" s="8"/>
+      <c r="AN7" s="9"/>
     </row>
     <row r="8" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -1574,19 +1653,19 @@
         <f t="shared" si="16"/>
         <v>400</v>
       </c>
-      <c r="AJ8" s="12">
+      <c r="AJ8" s="7">
         <v>24</v>
       </c>
-      <c r="AK8" s="7">
+      <c r="AK8" s="15">
         <v>25</v>
       </c>
-      <c r="AL8" s="7">
+      <c r="AL8" s="15">
         <v>26</v>
       </c>
-      <c r="AM8" s="4">
+      <c r="AM8" s="13">
         <v>27</v>
       </c>
-      <c r="AN8" s="8"/>
+      <c r="AN8" s="9"/>
     </row>
     <row r="9" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -1717,12 +1796,12 @@
         <f t="shared" si="16"/>
         <v>399</v>
       </c>
-      <c r="AJ9" s="8">
+      <c r="AJ9" s="16">
         <v>4</v>
       </c>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="8"/>
-      <c r="AM9" s="8"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="16"/>
     </row>
     <row r="10" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -1853,19 +1932,19 @@
         <f t="shared" si="16"/>
         <v>368</v>
       </c>
-      <c r="AJ10" s="10">
+      <c r="AJ10" s="5">
         <v>0</v>
       </c>
-      <c r="AK10" s="14">
+      <c r="AK10" s="11">
         <v>1</v>
       </c>
-      <c r="AL10" s="14">
+      <c r="AL10" s="11">
         <v>2</v>
       </c>
-      <c r="AM10" s="9">
+      <c r="AM10" s="12">
         <v>3</v>
       </c>
-      <c r="AN10" s="8">
+      <c r="AN10" s="9">
         <v>7</v>
       </c>
     </row>
@@ -1998,11 +2077,13 @@
         <f t="shared" si="16"/>
         <v>367</v>
       </c>
-      <c r="AJ11" s="10">
+      <c r="AJ11" s="5">
         <v>4</v>
       </c>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="8"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="9"/>
     </row>
     <row r="12" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -2134,10 +2215,10 @@
         <v>336</v>
       </c>
       <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="8"/>
+      <c r="AK12" s="13"/>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+      <c r="AN12" s="9"/>
     </row>
     <row r="13" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -2269,8 +2350,10 @@
         <v>335</v>
       </c>
       <c r="AJ13" s="4"/>
-      <c r="AM13" s="4"/>
-      <c r="AN13" s="8"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="13"/>
+      <c r="AN13" s="9"/>
     </row>
     <row r="14" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -2402,8 +2485,10 @@
         <v>304</v>
       </c>
       <c r="AJ14" s="4"/>
+      <c r="AK14" s="13"/>
+      <c r="AL14" s="13"/>
       <c r="AM14" s="4"/>
-      <c r="AN14" s="8"/>
+      <c r="AN14" s="9"/>
     </row>
     <row r="15" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -2535,10 +2620,12 @@
         <v>303</v>
       </c>
       <c r="AJ15" s="4"/>
+      <c r="AK15" s="13"/>
+      <c r="AL15" s="13"/>
       <c r="AM15" s="4">
         <v>23</v>
       </c>
-      <c r="AN15" s="8"/>
+      <c r="AN15" s="9"/>
     </row>
     <row r="16" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
@@ -2669,19 +2756,19 @@
         <f t="shared" si="16"/>
         <v>272</v>
       </c>
-      <c r="AJ16" s="2">
+      <c r="AJ16" s="7">
         <v>24</v>
       </c>
-      <c r="AK16" s="13">
+      <c r="AK16" s="8">
         <v>25</v>
       </c>
-      <c r="AL16" s="13">
+      <c r="AL16" s="8">
         <v>26</v>
       </c>
-      <c r="AM16">
+      <c r="AM16" s="13">
         <v>27</v>
       </c>
-      <c r="AN16" s="8"/>
+      <c r="AN16" s="9"/>
     </row>
     <row r="17" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -2950,12 +3037,12 @@
     <mergeCell ref="AN10:AN16"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:Q17 S2:AH17">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$W$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2969,7 +3056,7 @@
   <dimension ref="A1:AN30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AJ8" sqref="AJ8"/>
+      <selection activeCell="AP10" sqref="AP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,7 +3218,7 @@
         <f t="shared" si="8"/>
         <v>271</v>
       </c>
-      <c r="AJ2" s="6">
+      <c r="AJ2" s="10">
         <v>0</v>
       </c>
       <c r="AK2" s="11">
@@ -3140,10 +3227,10 @@
       <c r="AL2" s="11">
         <v>2</v>
       </c>
-      <c r="AM2" s="5">
+      <c r="AM2" s="12">
         <v>3</v>
       </c>
-      <c r="AN2" s="8">
+      <c r="AN2" s="9">
         <v>7</v>
       </c>
     </row>
@@ -3279,8 +3366,10 @@
       <c r="AJ3" s="10">
         <v>4</v>
       </c>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="8"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="9"/>
     </row>
     <row r="4" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -3411,9 +3500,11 @@
         <f t="shared" si="8"/>
         <v>269</v>
       </c>
-      <c r="AJ4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="8"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="9"/>
     </row>
     <row r="5" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -3544,9 +3635,11 @@
         <f t="shared" si="8"/>
         <v>268</v>
       </c>
-      <c r="AJ5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="8"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="9"/>
     </row>
     <row r="6" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -3677,11 +3770,11 @@
         <f t="shared" si="8"/>
         <v>267</v>
       </c>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="8"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="9"/>
     </row>
     <row r="7" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3812,11 +3905,13 @@
         <f t="shared" si="8"/>
         <v>266</v>
       </c>
-      <c r="AJ7" s="4"/>
-      <c r="AM7" s="4">
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13">
         <v>23</v>
       </c>
-      <c r="AN7" s="8"/>
+      <c r="AN7" s="9"/>
     </row>
     <row r="8" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -3947,19 +4042,19 @@
         <f t="shared" si="8"/>
         <v>265</v>
       </c>
-      <c r="AJ8" s="12">
+      <c r="AJ8" s="14">
         <v>24</v>
       </c>
-      <c r="AK8" s="7">
+      <c r="AK8" s="15">
         <v>25</v>
       </c>
-      <c r="AL8" s="7">
+      <c r="AL8" s="15">
         <v>26</v>
       </c>
-      <c r="AM8" s="4">
+      <c r="AM8" s="13">
         <v>27</v>
       </c>
-      <c r="AN8" s="8"/>
+      <c r="AN8" s="9"/>
     </row>
     <row r="9" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -4090,12 +4185,12 @@
         <f t="shared" si="8"/>
         <v>264</v>
       </c>
-      <c r="AJ9" s="8">
+      <c r="AJ9" s="9">
         <v>4</v>
       </c>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="8"/>
-      <c r="AM9" s="8"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -5232,7 +5327,7 @@
     <mergeCell ref="AJ9:AM9"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7451,7 +7546,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9665,11 +9760,1559 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$F$24</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D21C5-C0A1-4E54-8694-7F6956E417E2}">
+  <dimension ref="A1:AQ25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
+    <col min="19" max="34" width="5.140625" style="2" customWidth="1"/>
+    <col min="35" max="35" width="5.5703125" style="2" customWidth="1"/>
+    <col min="36" max="39" width="5.140625" style="2" customWidth="1"/>
+    <col min="40" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <f t="shared" ref="B2:O2" si="0">C2+1</f>
+        <v>255</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" si="0"/>
+        <v>246</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" si="0"/>
+        <v>245</v>
+      </c>
+      <c r="M2" s="1">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+      <c r="N2" s="1">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+      <c r="O2" s="1">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="P2" s="1">
+        <f>Q2+1</f>
+        <v>241</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>Q3+1</f>
+        <v>240</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>1</v>
+      </c>
+      <c r="U2" s="6">
+        <v>2</v>
+      </c>
+      <c r="V2" s="12">
+        <v>3</v>
+      </c>
+      <c r="W2" s="9">
+        <v>7</v>
+      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+    </row>
+    <row r="3" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <f>B4+1</f>
+        <v>224</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3+1</f>
+        <v>225</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:Q3" si="1">C3+1</f>
+        <v>226</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="1"/>
+        <v>229</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="1"/>
+        <v>231</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" si="1"/>
+        <v>232</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" si="1"/>
+        <v>233</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" si="1"/>
+        <v>234</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="1"/>
+        <v>235</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="1"/>
+        <v>236</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="1"/>
+        <v>237</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" si="1"/>
+        <v>238</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" si="1"/>
+        <v>239</v>
+      </c>
+      <c r="S3" s="5">
+        <v>4</v>
+      </c>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+    </row>
+    <row r="4" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:O4" si="2">C4+1</f>
+        <v>223</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="2"/>
+        <v>222</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="2"/>
+        <v>221</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="2"/>
+        <v>219</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="2"/>
+        <v>218</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="2"/>
+        <v>217</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>216</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="2"/>
+        <v>214</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="2"/>
+        <v>212</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="2"/>
+        <v>211</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="P4" s="1">
+        <f>Q4+1</f>
+        <v>209</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>Q5+1</f>
+        <v>208</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+    </row>
+    <row r="5" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <f>B6+1</f>
+        <v>192</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5+1</f>
+        <v>193</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:Q5" si="3">C5+1</f>
+        <v>194</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="3"/>
+        <v>199</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="1"/>
+      <c r="Z5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+    </row>
+    <row r="6" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:O6" si="4">C6+1</f>
+        <v>191</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="4"/>
+        <v>190</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="4"/>
+        <v>189</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="4"/>
+        <v>188</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="4"/>
+        <v>187</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="4"/>
+        <v>186</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="4"/>
+        <v>185</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="4"/>
+        <v>183</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="4"/>
+        <v>181</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>179</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="P6" s="1">
+        <f>Q6+1</f>
+        <v>177</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>Q7+1</f>
+        <v>176</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+    </row>
+    <row r="7" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <f>B8+1</f>
+        <v>160</v>
+      </c>
+      <c r="C7" s="1">
+        <f>B7+1</f>
+        <v>161</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:Q7" si="5">C7+1</f>
+        <v>162</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="5"/>
+        <v>163</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="5"/>
+        <v>165</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="5"/>
+        <v>166</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="5"/>
+        <v>167</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="5"/>
+        <v>169</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="5"/>
+        <v>171</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="5"/>
+        <v>172</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="5"/>
+        <v>173</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="5"/>
+        <v>174</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="5"/>
+        <v>175</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13">
+        <v>23</v>
+      </c>
+      <c r="W7" s="9"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+    </row>
+    <row r="8" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f t="shared" ref="B8:O8" si="6">C8+1</f>
+        <v>159</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="6"/>
+        <v>158</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="6"/>
+        <v>157</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="6"/>
+        <v>156</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="6"/>
+        <v>155</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="6"/>
+        <v>154</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="6"/>
+        <v>153</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="6"/>
+        <v>152</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="6"/>
+        <v>151</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="6"/>
+        <v>149</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="6"/>
+        <v>148</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="6"/>
+        <v>147</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="6"/>
+        <v>146</v>
+      </c>
+      <c r="P8" s="1">
+        <f>Q8+1</f>
+        <v>145</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>Q9+1</f>
+        <v>144</v>
+      </c>
+      <c r="S8" s="7">
+        <v>24</v>
+      </c>
+      <c r="T8" s="15">
+        <v>25</v>
+      </c>
+      <c r="U8" s="15">
+        <v>26</v>
+      </c>
+      <c r="V8" s="13">
+        <v>27</v>
+      </c>
+      <c r="W8" s="9"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+    </row>
+    <row r="9" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <f>B10+1</f>
+        <v>128</v>
+      </c>
+      <c r="C9" s="1">
+        <f>B9+1</f>
+        <v>129</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:Q9" si="7">C9+1</f>
+        <v>130</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="7"/>
+        <v>131</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="7"/>
+        <v>132</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="7"/>
+        <v>133</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="7"/>
+        <v>134</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="7"/>
+        <v>135</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="7"/>
+        <v>136</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="7"/>
+        <v>138</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="7"/>
+        <v>139</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="7"/>
+        <v>142</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="7"/>
+        <v>143</v>
+      </c>
+      <c r="S9" s="16">
+        <v>4</v>
+      </c>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+    </row>
+    <row r="10" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <f t="shared" ref="B10:O10" si="8">C10+1</f>
+        <v>127</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="8"/>
+        <v>126</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="8"/>
+        <v>125</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="8"/>
+        <v>124</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="8"/>
+        <v>123</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="8"/>
+        <v>122</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="8"/>
+        <v>121</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="8"/>
+        <v>120</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="8"/>
+        <v>119</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="8"/>
+        <v>118</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="8"/>
+        <v>117</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="8"/>
+        <v>116</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="8"/>
+        <v>115</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="8"/>
+        <v>114</v>
+      </c>
+      <c r="P10" s="1">
+        <f>Q10+1</f>
+        <v>113</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>Q11+1</f>
+        <v>112</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="11">
+        <v>1</v>
+      </c>
+      <c r="U10" s="11">
+        <v>2</v>
+      </c>
+      <c r="V10" s="12">
+        <v>3</v>
+      </c>
+      <c r="W10" s="9">
+        <v>7</v>
+      </c>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+    </row>
+    <row r="11" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <f>B12+1</f>
+        <v>96</v>
+      </c>
+      <c r="C11" s="1">
+        <f>B11+1</f>
+        <v>97</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" ref="D11:Q11" si="9">C11+1</f>
+        <v>98</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="9"/>
+        <v>102</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="9"/>
+        <v>103</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="9"/>
+        <v>104</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="9"/>
+        <v>106</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="9"/>
+        <v>107</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="9"/>
+        <v>108</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="9"/>
+        <v>109</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="9"/>
+        <v>110</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="9"/>
+        <v>111</v>
+      </c>
+      <c r="S11" s="5">
+        <v>4</v>
+      </c>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+    </row>
+    <row r="12" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <f t="shared" ref="B12:O12" si="10">C12+1</f>
+        <v>95</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="10"/>
+        <v>94</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="10"/>
+        <v>93</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="10"/>
+        <v>92</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="10"/>
+        <v>91</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="10"/>
+        <v>89</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="10"/>
+        <v>88</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="10"/>
+        <v>87</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="10"/>
+        <v>86</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="10"/>
+        <v>85</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="10"/>
+        <v>84</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="10"/>
+        <v>83</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="10"/>
+        <v>82</v>
+      </c>
+      <c r="P12" s="1">
+        <f>Q12+1</f>
+        <v>81</v>
+      </c>
+      <c r="Q12" s="1">
+        <f>Q13+1</f>
+        <v>80</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+    </row>
+    <row r="13" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <f>B14+1</f>
+        <v>64</v>
+      </c>
+      <c r="C13" s="1">
+        <f>B13+1</f>
+        <v>65</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:Q13" si="11">C13+1</f>
+        <v>66</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="11"/>
+        <v>67</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="11"/>
+        <v>68</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="11"/>
+        <v>69</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="11"/>
+        <v>71</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="11"/>
+        <v>73</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="11"/>
+        <v>74</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="11"/>
+        <v>76</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="11"/>
+        <v>77</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="11"/>
+        <v>79</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+    </row>
+    <row r="14" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <f t="shared" ref="B14:O16" si="12">C14+1</f>
+        <v>63</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="12"/>
+        <v>62</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="12"/>
+        <v>61</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="12"/>
+        <v>59</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="12"/>
+        <v>58</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="12"/>
+        <v>57</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="12"/>
+        <v>56</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="12"/>
+        <v>54</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="12"/>
+        <v>53</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="12"/>
+        <v>52</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="12"/>
+        <v>51</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="12"/>
+        <v>50</v>
+      </c>
+      <c r="P14" s="1">
+        <f>Q14+1</f>
+        <v>49</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>Q15+1</f>
+        <v>48</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+    </row>
+    <row r="15" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <f>B16+1</f>
+        <v>32</v>
+      </c>
+      <c r="C15" s="1">
+        <f>B15+1</f>
+        <v>33</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" ref="D15:Q15" si="13">C15+1</f>
+        <v>34</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="13"/>
+        <v>35</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="13"/>
+        <v>37</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="13"/>
+        <v>38</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="13"/>
+        <v>39</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="13"/>
+        <v>40</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="13"/>
+        <v>41</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="13"/>
+        <v>42</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="13"/>
+        <v>43</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="13"/>
+        <v>44</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="13"/>
+        <v>46</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="13"/>
+        <v>47</v>
+      </c>
+      <c r="S15" s="4"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="4">
+        <v>23</v>
+      </c>
+      <c r="W15" s="9"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+    </row>
+    <row r="16" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <f t="shared" si="12"/>
+        <v>31</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="12"/>
+        <v>29</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="12"/>
+        <v>28</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="12"/>
+        <v>27</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="12"/>
+        <v>26</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="12"/>
+        <v>23</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="12"/>
+        <v>22</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="12"/>
+        <v>21</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="12"/>
+        <v>19</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="P16" s="1">
+        <f>Q16+1</f>
+        <v>17</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>Q17+1</f>
+        <v>16</v>
+      </c>
+      <c r="S16" s="7">
+        <v>24</v>
+      </c>
+      <c r="T16" s="8">
+        <v>25</v>
+      </c>
+      <c r="U16" s="8">
+        <v>26</v>
+      </c>
+      <c r="V16" s="13">
+        <v>27</v>
+      </c>
+      <c r="W16" s="9"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+    </row>
+    <row r="17" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <f>B17+1</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" ref="D17:Q17" si="14">C17+1</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="O17" s="1">
+        <f>N17+1</f>
+        <v>13</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>28</v>
+      </c>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="S19"/>
+      <c r="T19" t="s">
+        <v>29</v>
+      </c>
+      <c r="U19"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="V24" s="3"/>
+    </row>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="S25" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="W2:W8"/>
+    <mergeCell ref="S9:V9"/>
+    <mergeCell ref="W10:W16"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2:Q17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>$F$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:Q17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$W$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mx completing excel fies about _StartongFrom0
</commit_message>
<xml_diff>
--- a/refFiles/mx_manip/posRecovery().xlsx
+++ b/refFiles/mx_manip/posRecovery().xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOUGNON-PEIGNE\Documents\_CodePro\SilProj\dev-ws2812b\refFiles\mx_manip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FilpUsine1\Documents\dev-ws2812b\refFiles\mx_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA8DCE0-793F-4FE8-A645-2D930A180135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F068DD-E06D-423F-82C5-4C095B830811}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
+    <workbookView xWindow="45" yWindow="630" windowWidth="38700" windowHeight="15435" activeTab="3" xr2:uid="{AA0145D3-E6E7-4C83-AE88-31E43BFD1697}"/>
   </bookViews>
   <sheets>
     <sheet name="0_360" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>Simple Matrix</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>MAX_LEDS - (MAX_COLU - (X - 1)) - (Y - 1) * MAX_COLU</t>
-  </si>
-  <si>
-    <t>Simplified in code !</t>
   </si>
   <si>
     <t>(X * MAX_LINE - 1) - (Y - 1)</t>
@@ -227,9 +224,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -246,17 +240,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -327,26 +324,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -361,7 +338,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -663,7 +640,7 @@
       <selection activeCell="B2" sqref="B2:Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
@@ -829,14 +806,14 @@
       <c r="AL2" s="6">
         <v>2</v>
       </c>
-      <c r="AM2" s="12">
+      <c r="AM2" s="11">
         <v>3</v>
       </c>
-      <c r="AN2" s="9">
+      <c r="AN2" s="16">
         <v>7</v>
       </c>
       <c r="AO2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -971,12 +948,12 @@
       <c r="AJ3" s="5">
         <v>4</v>
       </c>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
       <c r="AM3" s="4"/>
-      <c r="AN3" s="9"/>
+      <c r="AN3" s="16"/>
       <c r="AP3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1109,12 +1086,12 @@
         <v>464</v>
       </c>
       <c r="AJ4" s="4"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
       <c r="AM4" s="4"/>
-      <c r="AN4" s="9"/>
+      <c r="AN4" s="16"/>
       <c r="AQ4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,8 +1226,8 @@
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="9"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="16"/>
     </row>
     <row r="6" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -1382,10 +1359,10 @@
         <v>432</v>
       </c>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="13"/>
-      <c r="AM6" s="13"/>
-      <c r="AN6" s="9"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="16"/>
     </row>
     <row r="7" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -1517,12 +1494,12 @@
         <v>431</v>
       </c>
       <c r="AJ7" s="4"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="13"/>
-      <c r="AM7" s="13">
+      <c r="AK7" s="12"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="12">
         <v>23</v>
       </c>
-      <c r="AN7" s="9"/>
+      <c r="AN7" s="16"/>
     </row>
     <row r="8" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -1656,16 +1633,16 @@
       <c r="AJ8" s="7">
         <v>24</v>
       </c>
-      <c r="AK8" s="15">
+      <c r="AK8" s="14">
         <v>25</v>
       </c>
-      <c r="AL8" s="15">
+      <c r="AL8" s="14">
         <v>26</v>
       </c>
-      <c r="AM8" s="13">
+      <c r="AM8" s="12">
         <v>27</v>
       </c>
-      <c r="AN8" s="9"/>
+      <c r="AN8" s="16"/>
     </row>
     <row r="9" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -1796,12 +1773,12 @@
         <f t="shared" si="16"/>
         <v>399</v>
       </c>
-      <c r="AJ9" s="16">
+      <c r="AJ9" s="17">
         <v>4</v>
       </c>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
-      <c r="AM9" s="16"/>
+      <c r="AK9" s="17"/>
+      <c r="AL9" s="17"/>
+      <c r="AM9" s="17"/>
     </row>
     <row r="10" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -1935,16 +1912,16 @@
       <c r="AJ10" s="5">
         <v>0</v>
       </c>
-      <c r="AK10" s="11">
+      <c r="AK10" s="10">
         <v>1</v>
       </c>
-      <c r="AL10" s="11">
+      <c r="AL10" s="10">
         <v>2</v>
       </c>
-      <c r="AM10" s="12">
+      <c r="AM10" s="11">
         <v>3</v>
       </c>
-      <c r="AN10" s="9">
+      <c r="AN10" s="16">
         <v>7</v>
       </c>
     </row>
@@ -2080,10 +2057,10 @@
       <c r="AJ11" s="5">
         <v>4</v>
       </c>
-      <c r="AK11" s="13"/>
-      <c r="AL11" s="13"/>
-      <c r="AM11" s="13"/>
-      <c r="AN11" s="9"/>
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="12"/>
+      <c r="AM11" s="12"/>
+      <c r="AN11" s="16"/>
     </row>
     <row r="12" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -2215,10 +2192,10 @@
         <v>336</v>
       </c>
       <c r="AJ12" s="4"/>
-      <c r="AK12" s="13"/>
-      <c r="AL12" s="13"/>
-      <c r="AM12" s="13"/>
-      <c r="AN12" s="9"/>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="12"/>
+      <c r="AN12" s="16"/>
     </row>
     <row r="13" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -2352,8 +2329,8 @@
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
-      <c r="AM13" s="13"/>
-      <c r="AN13" s="9"/>
+      <c r="AM13" s="12"/>
+      <c r="AN13" s="16"/>
     </row>
     <row r="14" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -2485,10 +2462,10 @@
         <v>304</v>
       </c>
       <c r="AJ14" s="4"/>
-      <c r="AK14" s="13"/>
-      <c r="AL14" s="13"/>
+      <c r="AK14" s="12"/>
+      <c r="AL14" s="12"/>
       <c r="AM14" s="4"/>
-      <c r="AN14" s="9"/>
+      <c r="AN14" s="16"/>
     </row>
     <row r="15" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -2620,12 +2597,12 @@
         <v>303</v>
       </c>
       <c r="AJ15" s="4"/>
-      <c r="AK15" s="13"/>
-      <c r="AL15" s="13"/>
+      <c r="AK15" s="12"/>
+      <c r="AL15" s="12"/>
       <c r="AM15" s="4">
         <v>23</v>
       </c>
-      <c r="AN15" s="9"/>
+      <c r="AN15" s="16"/>
     </row>
     <row r="16" spans="2:43" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
@@ -2765,10 +2742,10 @@
       <c r="AL16" s="8">
         <v>26</v>
       </c>
-      <c r="AM16" s="13">
+      <c r="AM16" s="12">
         <v>27</v>
       </c>
-      <c r="AN16" s="9"/>
+      <c r="AN16" s="16"/>
     </row>
     <row r="17" spans="2:34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -3059,7 +3036,7 @@
       <selection activeCell="AP10" sqref="AP10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
@@ -3218,19 +3195,19 @@
         <f t="shared" si="8"/>
         <v>271</v>
       </c>
-      <c r="AJ2" s="10">
+      <c r="AJ2" s="9">
         <v>0</v>
       </c>
-      <c r="AK2" s="11">
+      <c r="AK2" s="10">
         <v>1</v>
       </c>
-      <c r="AL2" s="11">
+      <c r="AL2" s="10">
         <v>2</v>
       </c>
-      <c r="AM2" s="12">
+      <c r="AM2" s="11">
         <v>3</v>
       </c>
-      <c r="AN2" s="9">
+      <c r="AN2" s="16">
         <v>7</v>
       </c>
     </row>
@@ -3363,13 +3340,13 @@
         <f t="shared" si="8"/>
         <v>270</v>
       </c>
-      <c r="AJ3" s="10">
+      <c r="AJ3" s="9">
         <v>4</v>
       </c>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13"/>
-      <c r="AM3" s="13"/>
-      <c r="AN3" s="9"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="16"/>
     </row>
     <row r="4" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -3500,11 +3477,11 @@
         <f t="shared" si="8"/>
         <v>269</v>
       </c>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
-      <c r="AM4" s="13"/>
-      <c r="AN4" s="9"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="16"/>
     </row>
     <row r="5" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -3635,11 +3612,11 @@
         <f t="shared" si="8"/>
         <v>268</v>
       </c>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="13"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="9"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="16"/>
     </row>
     <row r="6" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -3770,11 +3747,11 @@
         <f t="shared" si="8"/>
         <v>267</v>
       </c>
-      <c r="AJ6" s="13"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="13"/>
-      <c r="AM6" s="13"/>
-      <c r="AN6" s="9"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="16"/>
     </row>
     <row r="7" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3905,13 +3882,13 @@
         <f t="shared" si="8"/>
         <v>266</v>
       </c>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="13"/>
-      <c r="AM7" s="13">
+      <c r="AJ7" s="12"/>
+      <c r="AK7" s="12"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="12">
         <v>23</v>
       </c>
-      <c r="AN7" s="9"/>
+      <c r="AN7" s="16"/>
     </row>
     <row r="8" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -4042,19 +4019,19 @@
         <f t="shared" si="8"/>
         <v>265</v>
       </c>
-      <c r="AJ8" s="14">
+      <c r="AJ8" s="13">
         <v>24</v>
       </c>
-      <c r="AK8" s="15">
+      <c r="AK8" s="14">
         <v>25</v>
       </c>
-      <c r="AL8" s="15">
+      <c r="AL8" s="14">
         <v>26</v>
       </c>
-      <c r="AM8" s="13">
+      <c r="AM8" s="12">
         <v>27</v>
       </c>
-      <c r="AN8" s="9"/>
+      <c r="AN8" s="16"/>
     </row>
     <row r="9" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -4185,12 +4162,12 @@
         <f t="shared" si="8"/>
         <v>264</v>
       </c>
-      <c r="AJ9" s="9">
+      <c r="AJ9" s="16">
         <v>4</v>
       </c>
-      <c r="AK9" s="9"/>
-      <c r="AL9" s="9"/>
-      <c r="AM9" s="9"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="16"/>
     </row>
     <row r="10" spans="2:40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -5338,13 +5315,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688FCD4D-605E-4791-BC54-A6D9EB8A5096}">
-  <dimension ref="A1:AH33"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
@@ -7539,11 +7516,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:Q17">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -7559,11 +7531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF87678-2DC5-468A-BDD2-E206238D660F}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
@@ -9745,7 +9717,7 @@
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.25">
@@ -9755,7 +9727,7 @@
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -9773,11 +9745,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D21C5-C0A1-4E54-8694-7F6956E417E2}">
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="17" width="5.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.5703125" style="2" customWidth="1"/>
@@ -9879,15 +9851,15 @@
       <c r="U2" s="6">
         <v>2</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="11">
         <v>3</v>
       </c>
-      <c r="W2" s="9">
+      <c r="W2" s="16">
         <v>7</v>
       </c>
       <c r="X2" s="1"/>
-      <c r="Y2" s="17" t="s">
-        <v>31</v>
+      <c r="Y2" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
@@ -9975,14 +9947,14 @@
       <c r="S3" s="5">
         <v>4</v>
       </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="4"/>
-      <c r="W3" s="9"/>
+      <c r="W3" s="16"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -10067,14 +10039,14 @@
         <v>208</v>
       </c>
       <c r="S4" s="4"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
       <c r="V4" s="4"/>
-      <c r="W4" s="9"/>
+      <c r="W4" s="16"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -10161,11 +10133,11 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="9"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="16"/>
       <c r="X5" s="1"/>
       <c r="Z5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -10249,14 +10221,14 @@
         <v>176</v>
       </c>
       <c r="S6" s="4"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="9"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="16"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
@@ -10338,12 +10310,12 @@
         <v>175</v>
       </c>
       <c r="S7" s="4"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13">
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12">
         <v>23</v>
       </c>
-      <c r="W7" s="9"/>
+      <c r="W7" s="16"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
@@ -10429,16 +10401,16 @@
       <c r="S8" s="7">
         <v>24</v>
       </c>
-      <c r="T8" s="15">
+      <c r="T8" s="14">
         <v>25</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U8" s="14">
         <v>26</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>27</v>
       </c>
-      <c r="W8" s="9"/>
+      <c r="W8" s="16"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
@@ -10521,12 +10493,12 @@
         <f t="shared" si="7"/>
         <v>143</v>
       </c>
-      <c r="S9" s="16">
+      <c r="S9" s="17">
         <v>4</v>
       </c>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -10612,16 +10584,16 @@
       <c r="S10" s="5">
         <v>0</v>
       </c>
-      <c r="T10" s="11">
+      <c r="T10" s="10">
         <v>1</v>
       </c>
-      <c r="U10" s="11">
+      <c r="U10" s="10">
         <v>2</v>
       </c>
-      <c r="V10" s="12">
+      <c r="V10" s="11">
         <v>3</v>
       </c>
-      <c r="W10" s="9">
+      <c r="W10" s="16">
         <v>7</v>
       </c>
       <c r="X10" s="1"/>
@@ -10709,10 +10681,10 @@
       <c r="S11" s="5">
         <v>4</v>
       </c>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="9"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="16"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
@@ -10796,10 +10768,10 @@
         <v>80</v>
       </c>
       <c r="S12" s="4"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="9"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="16"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
@@ -10885,8 +10857,8 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="9"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="16"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
@@ -10970,10 +10942,10 @@
         <v>48</v>
       </c>
       <c r="S14" s="4"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
       <c r="V14" s="4"/>
-      <c r="W14" s="9"/>
+      <c r="W14" s="16"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
@@ -11057,12 +11029,12 @@
         <v>47</v>
       </c>
       <c r="S15" s="4"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
       <c r="V15" s="4">
         <v>23</v>
       </c>
-      <c r="W15" s="9"/>
+      <c r="W15" s="16"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
@@ -11154,10 +11126,10 @@
       <c r="U16" s="8">
         <v>26</v>
       </c>
-      <c r="V16" s="13">
+      <c r="V16" s="12">
         <v>27</v>
       </c>
-      <c r="W16" s="9"/>
+      <c r="W16" s="16"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
@@ -11258,7 +11230,7 @@
     </row>
     <row r="18" spans="2:34" x14ac:dyDescent="0.25">
       <c r="S18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T18"/>
       <c r="U18"/>
@@ -11270,7 +11242,7 @@
       <c r="G19" s="3"/>
       <c r="S19"/>
       <c r="T19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U19"/>
       <c r="V19" s="1"/>
@@ -11281,7 +11253,7 @@
       <c r="S20"/>
       <c r="T20"/>
       <c r="U20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>

</xml_diff>